<commit_message>
first final draft of CVA project
</commit_message>
<xml_diff>
--- a/finalProject/CVA/PD/my CDS Bootstrapping v2.xlsx
+++ b/finalProject/CVA/PD/my CDS Bootstrapping v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="13035" tabRatio="814"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="13035" tabRatio="814" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOOTSTRAP EXAMPLE" sheetId="18" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <definedName name="ST">#REF!</definedName>
     <definedName name="STRIKEVEC">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621" calcMode="manual" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>DF</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>DF(T, T+0.5)</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -188,8 +185,8 @@
     <numFmt numFmtId="167" formatCode="dd\ mmm\ yy"/>
     <numFmt numFmtId="168" formatCode="0.00000000"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000%"/>
-    <numFmt numFmtId="178" formatCode="0.0000000000000%"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000%"/>
+    <numFmt numFmtId="171" formatCode="0.0000000000000%"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -544,13 +541,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="175" fontId="10" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -794,11 +791,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75723136"/>
-        <c:axId val="75725056"/>
+        <c:axId val="72754304"/>
+        <c:axId val="72756224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75723136"/>
+        <c:axId val="72754304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -829,13 +826,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75725056"/>
+        <c:crossAx val="72756224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75725056"/>
+        <c:axId val="72756224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75723136"/>
+        <c:crossAx val="72754304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1006,11 +1003,11 @@
         </c:dLbls>
         <c:gapWidth val="8"/>
         <c:overlap val="-10"/>
-        <c:axId val="85994496"/>
-        <c:axId val="134907776"/>
+        <c:axId val="72764032"/>
+        <c:axId val="72798976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="85994496"/>
+        <c:axId val="72764032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1039,7 +1036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134907776"/>
+        <c:crossAx val="72798976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1047,7 +1044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134907776"/>
+        <c:axId val="72798976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +1055,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85994496"/>
+        <c:crossAx val="72764032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1332,11 +1329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="141372800"/>
-        <c:axId val="142658944"/>
+        <c:axId val="80819328"/>
+        <c:axId val="80821248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="141372800"/>
+        <c:axId val="80819328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1367,12 +1364,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142658944"/>
+        <c:crossAx val="80821248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="142658944"/>
+        <c:axId val="80821248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141372800"/>
+        <c:crossAx val="80819328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1808,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2849,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:L9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3095,8 +3092,9 @@
       <c r="A9" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>50</v>
+      <c r="B9" s="35">
+        <f>B8</f>
+        <v>1</v>
       </c>
       <c r="C9" s="35">
         <f>C8/B8</f>

</xml_diff>

<commit_message>
fixed calculation of DF (now calculated per simulation) and then taking avg, CDS Bootstrapping file required updating to this DF to get updated PDs
</commit_message>
<xml_diff>
--- a/finalProject/CVA/PD/my CDS Bootstrapping v2.xlsx
+++ b/finalProject/CVA/PD/my CDS Bootstrapping v2.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="13035" tabRatio="814" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14400" windowHeight="12855" tabRatio="814"/>
   </bookViews>
   <sheets>
     <sheet name="BOOTSTRAP EXAMPLE" sheetId="18" r:id="rId1"/>
-    <sheet name="DF" sheetId="19" r:id="rId2"/>
+    <sheet name="input" sheetId="20" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="dt">'BOOTSTRAP EXAMPLE'!$B$11</definedName>
@@ -16,12 +16,12 @@
     <definedName name="ST">#REF!</definedName>
     <definedName name="STRIKEVEC">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>DF</t>
   </si>
@@ -86,21 +86,6 @@
     <t>30Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Maturity </t>
-  </si>
-  <si>
-    <t>months:</t>
-  </si>
-  <si>
-    <t>years:</t>
-  </si>
-  <si>
-    <t>Taken from BoE OIS spot curve</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>1st term</t>
   </si>
   <si>
@@ -167,28 +152,26 @@
     <t>P_cum</t>
   </si>
   <si>
-    <t>DF(0, T)</t>
-  </si>
-  <si>
-    <t>DF(T, T+0.5)</t>
+    <t>Tenor</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="dd\ mmm\ yy"/>
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.0000000000%"/>
-    <numFmt numFmtId="171" formatCode="0.0000000000000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000%"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000000%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -211,14 +194,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -232,12 +207,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -274,7 +243,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,14 +285,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -381,21 +344,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -425,143 +373,111 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8"/>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="6" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="5" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="8" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="7"/>
-    <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Comma 2" xfId="6"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 2 2" xfId="9"/>
-    <cellStyle name="Normal 2 3" xfId="8"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Percent" xfId="4" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 2 2" xfId="8"/>
+    <cellStyle name="Normal 2 3" xfId="7"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -752,31 +668,31 @@
                   <c:v>9.4433071386118561E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.250518150293134E-2</c:v>
+                  <c:v>1.2509564610413304E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8864387026094831E-2</c:v>
+                  <c:v>1.8886540726516965E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3832815903738647E-2</c:v>
+                  <c:v>2.3875123521640451E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8509922892786532E-2</c:v>
+                  <c:v>2.8578590499201306E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2874818742636869E-2</c:v>
+                  <c:v>3.2974468454083694E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4658008104643034E-2</c:v>
+                  <c:v>3.4775856267641569E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.7793749030792023E-2</c:v>
+                  <c:v>3.7947249524283966E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9425351524786989E-2</c:v>
+                  <c:v>3.9604742054686115E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1696931324958331E-2</c:v>
+                  <c:v>4.1914099356345047E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,11 +707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72754304"/>
-        <c:axId val="72756224"/>
+        <c:axId val="119377920"/>
+        <c:axId val="119379840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72754304"/>
+        <c:axId val="119377920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -826,13 +742,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72756224"/>
+        <c:crossAx val="119379840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72756224"/>
+        <c:axId val="119379840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +759,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72754304"/>
+        <c:crossAx val="119377920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -963,31 +879,31 @@
                   <c:v>1.8976355744616674E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2192940233669186E-2</c:v>
+                  <c:v>2.2197421712663361E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7779399132555064E-2</c:v>
+                  <c:v>2.7797843343853341E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3414940988517092E-2</c:v>
+                  <c:v>3.3451743598432469E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9113765643875281E-2</c:v>
+                  <c:v>3.9174425426960563E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.490324151186631E-2</c:v>
+                  <c:v>4.4993707639747055E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0049513190899723E-2</c:v>
+                  <c:v>5.0170389471591678E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5312021692614927E-2</c:v>
+                  <c:v>5.5470680605277427E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0374976560801562E-2</c:v>
+                  <c:v>6.0575655501680231E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.5590975003326585E-2</c:v>
+                  <c:v>6.5842402988677398E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1003,11 +919,11 @@
         </c:dLbls>
         <c:gapWidth val="8"/>
         <c:overlap val="-10"/>
-        <c:axId val="72764032"/>
-        <c:axId val="72798976"/>
+        <c:axId val="119547392"/>
+        <c:axId val="119549312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72764032"/>
+        <c:axId val="119547392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72798976"/>
+        <c:crossAx val="119549312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1044,7 +960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72798976"/>
+        <c:axId val="119549312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +971,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72764032"/>
+        <c:crossAx val="119547392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1190,31 +1106,31 @@
                   <c:v>9.4433071386118561E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1948488641543196E-2</c:v>
+                  <c:v>2.195287174902516E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0812875667638027E-2</c:v>
+                  <c:v>4.0839412475542125E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.4645691571376673E-2</c:v>
+                  <c:v>6.4714535997182576E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3155614464163206E-2</c:v>
+                  <c:v>9.3293126496383882E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12603043320680007</c:v>
+                  <c:v>0.12626759495046758</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16068844131144311</c:v>
+                  <c:v>0.16104345121810915</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.19848219034223513</c:v>
+                  <c:v>0.19899070074239311</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23790754186702212</c:v>
+                  <c:v>0.23859544279707923</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.27960447319198045</c:v>
+                  <c:v>0.28050954215342427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,31 +1206,31 @@
                   <c:v>0.99055669286138814</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9780515113584568</c:v>
+                  <c:v>0.97804712825097484</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95918712433236197</c:v>
+                  <c:v>0.95916058752445787</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93535430842862333</c:v>
+                  <c:v>0.93528546400281742</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.90684438553583679</c:v>
+                  <c:v>0.90670687350361612</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87396956679319993</c:v>
+                  <c:v>0.87373240504953242</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83931155868855689</c:v>
+                  <c:v>0.83895654878189085</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80151780965776487</c:v>
+                  <c:v>0.80100929925760689</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.76209245813297788</c:v>
+                  <c:v>0.76140455720292077</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.72039552680801955</c:v>
+                  <c:v>0.71949045784657573</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1329,11 +1245,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80819328"/>
-        <c:axId val="80821248"/>
+        <c:axId val="119578624"/>
+        <c:axId val="119580544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80819328"/>
+        <c:axId val="119578624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1364,12 +1280,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80821248"/>
+        <c:crossAx val="119580544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80821248"/>
+        <c:axId val="119580544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,7 +1296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80819328"/>
+        <c:crossAx val="119578624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1805,902 +1721,902 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="8" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" style="8" customWidth="1"/>
-    <col min="4" max="5" width="23.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="15" style="8" customWidth="1"/>
-    <col min="12" max="17" width="16" style="8" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="8" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" style="8" customWidth="1"/>
-    <col min="20" max="21" width="15.28515625" style="8" customWidth="1"/>
-    <col min="22" max="25" width="11.42578125" style="8"/>
-    <col min="26" max="26" width="20.28515625" style="24" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="16.5703125" style="4" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" style="4" customWidth="1"/>
+    <col min="4" max="5" width="23.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15" style="4" customWidth="1"/>
+    <col min="12" max="17" width="16" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" style="4" customWidth="1"/>
+    <col min="20" max="21" width="15.28515625" style="4" customWidth="1"/>
+    <col min="22" max="25" width="11.42578125" style="4"/>
+    <col min="26" max="26" width="20.28515625" style="20" customWidth="1"/>
+    <col min="27" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>46</v>
+      <c r="F7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
     </row>
     <row r="9" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="O9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="P9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="Q9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="11" t="s">
+      <c r="R9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S9" s="11" t="s">
+      <c r="S9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="T9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="U9" s="11" t="s">
+      <c r="U9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="12">
         <v>0</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15">
         <v>1</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="42">
+      <c r="E10" s="27"/>
+      <c r="F10" s="28">
         <f>G10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="22">
         <f>1-H10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="23">
         <v>1</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
     </row>
     <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="17">
         <f>A10+B11</f>
         <v>0.5</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="18">
         <v>0.5</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="19">
         <v>114.4</v>
       </c>
-      <c r="D11" s="19">
-        <v>0.9978845064467694</v>
-      </c>
-      <c r="E11" s="41">
+      <c r="D11" s="15">
+        <v>0.99583479331400004</v>
+      </c>
+      <c r="E11" s="27">
         <f t="shared" ref="E11:E20" si="0">-LN(H11)/A11</f>
         <v>1.8976355744616674E-2</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="28">
         <f>H10-H11</f>
         <v>9.4433071386118561E-3</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="22">
         <f t="shared" ref="G11:G20" si="1">1-H11</f>
         <v>9.4433071386118561E-3</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="22">
         <f>(1-RR)/((1-RR)+B11*C11/10000)</f>
         <v>0.99055669286138814</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
     </row>
     <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="17">
         <f t="shared" ref="A12:A20" si="2">A11+B12</f>
         <v>1</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="13">
         <f>$B$11</f>
         <v>0.5</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="19">
         <v>133.77000000000001</v>
       </c>
-      <c r="D12" s="19">
-        <v>0.99574925087026533</v>
-      </c>
-      <c r="E12" s="41">
+      <c r="D12" s="15">
+        <v>0.99096300549399996</v>
+      </c>
+      <c r="E12" s="27">
         <f t="shared" si="0"/>
-        <v>2.2192940233669186E-2</v>
-      </c>
-      <c r="F12" s="42">
+        <v>2.2197421712663361E-2</v>
+      </c>
+      <c r="F12" s="28">
         <f t="shared" ref="F12:F20" si="3">H11-H12</f>
-        <v>1.250518150293134E-2</v>
-      </c>
-      <c r="G12" s="26">
+        <v>1.2509564610413304E-2</v>
+      </c>
+      <c r="G12" s="22">
         <f t="shared" si="1"/>
-        <v>2.1948488641543196E-2</v>
-      </c>
-      <c r="H12" s="26">
+        <v>2.195287174902516E-2</v>
+      </c>
+      <c r="H12" s="22">
         <f>T12+U12</f>
-        <v>0.9780515113584568</v>
-      </c>
-      <c r="I12" s="20">
+        <v>0.97804712825097484</v>
+      </c>
+      <c r="I12" s="16">
         <f t="shared" ref="I12:I20" si="4">($D$11*((1-RR)*$H$10-(1-RR+$B$11*C12/10000)*$H$11))</f>
-        <v>-9.5732464950182099E-4</v>
-      </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20">
+        <v>-9.5535824868716679E-4</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16">
         <f>SUM(I12:Q12)</f>
-        <v>-9.5732464950182099E-4</v>
-      </c>
-      <c r="S12" s="20">
+        <v>-9.5535824868716679E-4</v>
+      </c>
+      <c r="S12" s="16">
         <f t="shared" ref="S12:S20" si="5">(D12*((1-RR)+B12*C12/10000))</f>
-        <v>0.6041096193866049</v>
-      </c>
-      <c r="T12" s="20">
+        <v>0.60120585935864657</v>
+      </c>
+      <c r="T12" s="16">
         <f>R12/S12</f>
-        <v>-1.5846869819319551E-3</v>
-      </c>
-      <c r="U12" s="20">
+        <v>-1.5890700894138363E-3</v>
+      </c>
+      <c r="U12" s="16">
         <f t="shared" ref="U12:U20" si="6">H11*(1-RR)/(1-RR+B12*C12/10000)</f>
         <v>0.97963619834038873</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+    <row r="13" spans="1:21" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="13">
         <f t="shared" ref="B13:B20" si="7">$B$11</f>
         <v>0.5</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="25">
         <f>AVERAGE(C12,C14)</f>
         <v>167.18</v>
       </c>
-      <c r="D13" s="19">
-        <v>0.99313114696376492</v>
-      </c>
-      <c r="E13" s="41">
+      <c r="D13" s="15">
+        <v>0.98569666301900005</v>
+      </c>
+      <c r="E13" s="27">
         <f t="shared" si="0"/>
-        <v>2.7779399132555064E-2</v>
-      </c>
-      <c r="F13" s="43">
+        <v>2.7797843343853341E-2</v>
+      </c>
+      <c r="F13" s="29">
         <f t="shared" si="3"/>
-        <v>1.8864387026094831E-2</v>
-      </c>
-      <c r="G13" s="26">
+        <v>1.8886540726516965E-2</v>
+      </c>
+      <c r="G13" s="22">
         <f t="shared" si="1"/>
-        <v>4.0812875667638027E-2</v>
-      </c>
-      <c r="H13" s="28">
+        <v>4.0839412475542125E-2</v>
+      </c>
+      <c r="H13" s="24">
         <f>T13+U13</f>
-        <v>0.95918712433236197</v>
-      </c>
-      <c r="I13" s="20">
+        <v>0.95916058752445787</v>
+      </c>
+      <c r="I13" s="16">
         <f>($D$11*((1-RR)*$H$10-(1-RR+$B$11*C13/10000)*$H$11))</f>
-        <v>-2.6085490449512072E-3</v>
-      </c>
-      <c r="J13" s="20">
+        <v>-2.6031909326642974E-3</v>
+      </c>
+      <c r="J13" s="16">
         <f t="shared" ref="J13:J20" si="8">($D$12*((1-RR)*$H$11-(1-RR+$B$12*C13/10000)*$H$12))</f>
-        <v>-6.6956537730677621E-4</v>
-      </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20">
+        <v>-6.6370458685672379E-4</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16">
         <f t="shared" ref="R13:R20" si="9">SUM(I13:Q13)</f>
-        <v>-3.2781144222579833E-3</v>
-      </c>
-      <c r="S13" s="20">
+        <v>-3.2668955195210214E-3</v>
+      </c>
+      <c r="S13" s="16">
         <f t="shared" si="5"/>
-        <v>0.60418027143572905</v>
-      </c>
-      <c r="T13" s="20">
+        <v>0.59965743621757583</v>
+      </c>
+      <c r="T13" s="16">
         <f>R13/S13</f>
-        <v>-5.4257223832683511E-3</v>
-      </c>
-      <c r="U13" s="20">
+        <v>-5.4479363086488639E-3</v>
+      </c>
+      <c r="U13" s="16">
         <f t="shared" si="6"/>
-        <v>0.9646128467156303</v>
+        <v>0.96460852383310669</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="17">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="19">
         <v>200.59</v>
       </c>
-      <c r="D14" s="19">
-        <v>0.99001269228735078</v>
-      </c>
-      <c r="E14" s="41">
+      <c r="D14" s="15">
+        <v>0.98010503953600003</v>
+      </c>
+      <c r="E14" s="27">
         <f t="shared" si="0"/>
-        <v>3.3414940988517092E-2</v>
-      </c>
-      <c r="F14" s="42">
+        <v>3.3451743598432469E-2</v>
+      </c>
+      <c r="F14" s="28">
         <f t="shared" si="3"/>
-        <v>2.3832815903738647E-2</v>
-      </c>
-      <c r="G14" s="26">
+        <v>2.3875123521640451E-2</v>
+      </c>
+      <c r="G14" s="22">
         <f t="shared" si="1"/>
-        <v>6.4645691571376673E-2</v>
-      </c>
-      <c r="H14" s="26">
+        <v>6.4714535997182576E-2</v>
+      </c>
+      <c r="H14" s="22">
         <f>T14+U14</f>
-        <v>0.93535430842862333</v>
-      </c>
-      <c r="I14" s="20">
+        <v>0.93528546400281742</v>
+      </c>
+      <c r="I14" s="16">
         <f t="shared" si="4"/>
-        <v>-4.2597734404005941E-3</v>
-      </c>
-      <c r="J14" s="20">
+        <v>-4.2510236166414285E-3</v>
+      </c>
+      <c r="J14" s="16">
         <f t="shared" si="8"/>
-        <v>-2.2964554041153941E-3</v>
-      </c>
-      <c r="K14" s="20">
+        <v>-2.2827674224005887E-3</v>
+      </c>
+      <c r="K14" s="16">
         <f t="shared" ref="K14:K20" si="10">($D$13*((1-RR)*$H$12-(1-RR+$B$13*C14/10000)*$H$13))</f>
-        <v>1.6867984460219028E-3</v>
-      </c>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20">
+        <v>1.687535676820672E-3</v>
+      </c>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16">
         <f t="shared" si="9"/>
-        <v>-4.8694303984940859E-3</v>
-      </c>
-      <c r="S14" s="20">
+        <v>-4.8462553622213448E-3</v>
+      </c>
+      <c r="S14" s="16">
         <f t="shared" si="5"/>
-        <v>0.6039369476697064</v>
-      </c>
-      <c r="T14" s="20">
+        <v>0.59789298721562634</v>
+      </c>
+      <c r="T14" s="16">
         <f>R14/S14</f>
-        <v>-8.0628125457182353E-3</v>
-      </c>
-      <c r="U14" s="20">
+        <v>-8.1055564554958943E-3</v>
+      </c>
+      <c r="U14" s="16">
         <f t="shared" si="6"/>
-        <v>0.94341712097434161</v>
+        <v>0.94339102045831336</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="17">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="25">
         <f>AVERAGE(C14,C16)</f>
         <v>233.96499999999997</v>
       </c>
-      <c r="D15" s="19">
-        <v>0.98647955260389597</v>
-      </c>
-      <c r="E15" s="41">
+      <c r="D15" s="15">
+        <v>0.97410111162099999</v>
+      </c>
+      <c r="E15" s="27">
         <f t="shared" si="0"/>
-        <v>3.9113765643875281E-2</v>
-      </c>
-      <c r="F15" s="43">
+        <v>3.9174425426960563E-2</v>
+      </c>
+      <c r="F15" s="29">
         <f t="shared" si="3"/>
-        <v>2.8509922892786532E-2</v>
-      </c>
-      <c r="G15" s="26">
+        <v>2.8578590499201306E-2</v>
+      </c>
+      <c r="G15" s="22">
         <f t="shared" si="1"/>
-        <v>9.3155614464163206E-2</v>
-      </c>
-      <c r="H15" s="28">
+        <v>9.3293126496383882E-2</v>
+      </c>
+      <c r="H15" s="24">
         <f>T15+U15</f>
-        <v>0.90684438553583679</v>
-      </c>
-      <c r="I15" s="20">
+        <v>0.90670687350361612</v>
+      </c>
+      <c r="I15" s="16">
         <f t="shared" si="4"/>
-        <v>-5.9092680287909953E-3</v>
-      </c>
-      <c r="J15" s="20">
+        <v>-5.8971300466844328E-3</v>
+      </c>
+      <c r="J15" s="16">
         <f t="shared" si="8"/>
-        <v>-3.921641116319383E-3</v>
-      </c>
-      <c r="K15" s="20">
+        <v>-3.9001341430314543E-3</v>
+      </c>
+      <c r="K15" s="16">
         <f t="shared" si="10"/>
-        <v>9.7149517351432217E-5</v>
-      </c>
-      <c r="L15" s="20">
+        <v>1.0983035655362996E-4</v>
+      </c>
+      <c r="L15" s="16">
         <f t="shared" ref="L15:L20" si="11">($D$14*((1-RR)*$H$13-(1-RR+$B$14*C15/10000)*$H$14))</f>
-        <v>3.3241468102834073E-3</v>
-      </c>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20">
+        <v>3.31654895527178E-3</v>
+      </c>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16">
         <f t="shared" si="9"/>
-        <v>-6.4096128174755381E-3</v>
-      </c>
-      <c r="S15" s="20">
+        <v>-6.3708848778904767E-3</v>
+      </c>
+      <c r="S15" s="16">
         <f t="shared" si="5"/>
-        <v>0.60342781598858608</v>
-      </c>
-      <c r="T15" s="20">
+        <v>0.59585594530162034</v>
+      </c>
+      <c r="T15" s="16">
         <f>R15/S15</f>
-        <v>-1.0622004235874961E-2</v>
-      </c>
-      <c r="U15" s="20">
+        <v>-1.0691988438020125E-2</v>
+      </c>
+      <c r="U15" s="16">
         <f t="shared" si="6"/>
-        <v>0.9174663897717118</v>
+        <v>0.91739886194163622</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="17">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="19">
         <v>267.33999999999997</v>
       </c>
-      <c r="D16" s="19">
-        <v>0.98258123599502745</v>
-      </c>
-      <c r="E16" s="41">
+      <c r="D16" s="15">
+        <v>0.96783236118000004</v>
+      </c>
+      <c r="E16" s="27">
         <f t="shared" si="0"/>
-        <v>4.490324151186631E-2</v>
-      </c>
-      <c r="F16" s="42">
+        <v>4.4993707639747055E-2</v>
+      </c>
+      <c r="F16" s="28">
         <f t="shared" si="3"/>
-        <v>3.2874818742636869E-2</v>
-      </c>
-      <c r="G16" s="26">
+        <v>3.2974468454083694E-2</v>
+      </c>
+      <c r="G16" s="22">
         <f t="shared" si="1"/>
-        <v>0.12603043320680007</v>
-      </c>
-      <c r="H16" s="26">
+        <v>0.12626759495046758</v>
+      </c>
+      <c r="H16" s="22">
         <f t="shared" ref="H16:H20" si="12">T16+U16</f>
-        <v>0.87396956679319993</v>
-      </c>
-      <c r="I16" s="20">
+        <v>0.87373240504953242</v>
+      </c>
+      <c r="I16" s="16">
         <f t="shared" si="4"/>
-        <v>-7.5587626171813964E-3</v>
-      </c>
-      <c r="J16" s="20">
+        <v>-7.5432364767274362E-3</v>
+      </c>
+      <c r="J16" s="16">
         <f t="shared" si="8"/>
-        <v>-5.5468268285233709E-3</v>
-      </c>
-      <c r="K16" s="20">
+        <v>-5.5175008636623203E-3</v>
+      </c>
+      <c r="K16" s="16">
         <f t="shared" si="10"/>
-        <v>-1.4924994113189279E-3</v>
-      </c>
-      <c r="L16" s="20">
+        <v>-1.4678749637134121E-3</v>
+      </c>
+      <c r="L16" s="16">
         <f t="shared" si="11"/>
-        <v>1.7788632220727141E-3</v>
-      </c>
-      <c r="M16" s="20">
+        <v>1.7868425483221237E-3</v>
+      </c>
+      <c r="M16" s="16">
         <f>($D$15*((1-RR)*$H$14-(1-RR+$B$15*C16/10000)*$H$15))</f>
-        <v>4.9167766957598702E-3</v>
-      </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20">
+        <v>4.8970045385387587E-3</v>
+      </c>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16">
         <f t="shared" si="9"/>
-        <v>-7.9024489391911097E-3</v>
-      </c>
-      <c r="S16" s="20">
+        <v>-7.8447652172422867E-3</v>
+      </c>
+      <c r="S16" s="16">
         <f t="shared" si="5"/>
-        <v>0.60268290497856203</v>
-      </c>
-      <c r="T16" s="20">
+        <v>0.59363643187989312</v>
+      </c>
+      <c r="T16" s="16">
         <f t="shared" ref="T16:T20" si="13">R16/S16</f>
-        <v>-1.3112117290720577E-2</v>
-      </c>
-      <c r="U16" s="20">
+        <v>-1.3214763777890017E-2</v>
+      </c>
+      <c r="U16" s="16">
         <f t="shared" si="6"/>
-        <v>0.88708168408392052</v>
+        <v>0.88694716882742242</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="17">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="25">
         <f>AVERAGE(C16,C18)</f>
         <v>296.54499999999996</v>
       </c>
-      <c r="D17" s="19">
-        <v>0.97831746958591959</v>
-      </c>
-      <c r="E17" s="41">
+      <c r="D17" s="15">
+        <v>0.96123247030000003</v>
+      </c>
+      <c r="E17" s="27">
         <f t="shared" si="0"/>
-        <v>5.0049513190899723E-2</v>
-      </c>
-      <c r="F17" s="43">
+        <v>5.0170389471591678E-2</v>
+      </c>
+      <c r="F17" s="29">
         <f t="shared" si="3"/>
-        <v>3.4658008104643034E-2</v>
-      </c>
-      <c r="G17" s="26">
+        <v>3.4775856267641569E-2</v>
+      </c>
+      <c r="G17" s="22">
         <f t="shared" si="1"/>
-        <v>0.16068844131144311</v>
-      </c>
-      <c r="H17" s="28">
+        <v>0.16104345121810915</v>
+      </c>
+      <c r="H17" s="24">
         <f t="shared" si="12"/>
-        <v>0.83931155868855689</v>
-      </c>
-      <c r="I17" s="20">
+        <v>0.83895654878189085</v>
+      </c>
+      <c r="I17" s="16">
         <f t="shared" si="4"/>
-        <v>-9.0021630502581437E-3</v>
-      </c>
-      <c r="J17" s="20">
+        <v>-8.983672080904238E-3</v>
+      </c>
+      <c r="J17" s="16">
         <f t="shared" si="8"/>
-        <v>-6.9689556292699606E-3</v>
-      </c>
-      <c r="K17" s="20">
+        <v>-6.9327876075131909E-3</v>
+      </c>
+      <c r="K17" s="16">
         <f t="shared" si="10"/>
-        <v>-2.8835315300250733E-3</v>
-      </c>
-      <c r="L17" s="20">
+        <v>-2.8484557540774283E-3</v>
+      </c>
+      <c r="L17" s="16">
         <f t="shared" si="11"/>
-        <v>4.266532687037688E-4</v>
-      </c>
-      <c r="M17" s="20">
+        <v>4.4826350367907795E-4</v>
+      </c>
+      <c r="M17" s="16">
         <f>($D$15*((1-RR)*$H$14-(1-RR+$B$15*C17/10000)*$H$15))</f>
-        <v>3.6104612220608603E-3</v>
-      </c>
-      <c r="N17" s="20">
+        <v>3.6072764393398427E-3</v>
+      </c>
+      <c r="N17" s="16">
         <f>($D$16*((1-RR)*$H$15-(1-RR+$B$16*C17/10000)*$H$16))</f>
-        <v>6.6484649508107294E-3</v>
-      </c>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20">
+        <v>6.6099391255550095E-3</v>
+      </c>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16">
         <f t="shared" si="9"/>
-        <v>-8.1690707679778173E-3</v>
-      </c>
-      <c r="S17" s="20">
+        <v>-8.099436373920927E-3</v>
+      </c>
+      <c r="S17" s="16">
         <f t="shared" si="5"/>
-        <v>0.60149623945246955</v>
-      </c>
-      <c r="T17" s="20">
+        <v>0.59099191632525561</v>
+      </c>
+      <c r="T17" s="16">
         <f t="shared" si="13"/>
-        <v>-1.3581249943331259E-2</v>
-      </c>
-      <c r="U17" s="20">
+        <v>-1.3704817528271162E-2</v>
+      </c>
+      <c r="U17" s="16">
         <f t="shared" si="6"/>
-        <v>0.8528928086318881</v>
+        <v>0.85266136631016198</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="17">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="19">
         <v>325.75</v>
       </c>
-      <c r="D18" s="19">
-        <v>0.97366043824697446</v>
-      </c>
-      <c r="E18" s="41">
+      <c r="D18" s="15">
+        <v>0.95423927873100001</v>
+      </c>
+      <c r="E18" s="27">
         <f t="shared" si="0"/>
-        <v>5.5312021692614927E-2</v>
-      </c>
-      <c r="F18" s="42">
+        <v>5.5470680605277427E-2</v>
+      </c>
+      <c r="F18" s="28">
         <f t="shared" si="3"/>
-        <v>3.7793749030792023E-2</v>
-      </c>
-      <c r="G18" s="26">
+        <v>3.7947249524283966E-2</v>
+      </c>
+      <c r="G18" s="22">
         <f t="shared" si="1"/>
-        <v>0.19848219034223513</v>
-      </c>
-      <c r="H18" s="26">
+        <v>0.19899070074239311</v>
+      </c>
+      <c r="H18" s="22">
         <f t="shared" si="12"/>
-        <v>0.80151780965776487</v>
-      </c>
-      <c r="I18" s="20">
+        <v>0.80100929925760689</v>
+      </c>
+      <c r="I18" s="16">
         <f t="shared" si="4"/>
-        <v>-1.0445563483335113E-2</v>
-      </c>
-      <c r="J18" s="20">
+        <v>-1.0424107685081259E-2</v>
+      </c>
+      <c r="J18" s="16">
         <f t="shared" si="8"/>
-        <v>-8.3910844300165502E-3</v>
-      </c>
-      <c r="K18" s="20">
+        <v>-8.3480743513641709E-3</v>
+      </c>
+      <c r="K18" s="16">
         <f t="shared" si="10"/>
-        <v>-4.2745636487313294E-3</v>
-      </c>
-      <c r="L18" s="20">
+        <v>-4.2290365444414444E-3</v>
+      </c>
+      <c r="L18" s="16">
         <f t="shared" si="11"/>
-        <v>-9.2555668466539633E-4</v>
-      </c>
-      <c r="M18" s="20">
+        <v>-8.9031554096407652E-4</v>
+      </c>
+      <c r="M18" s="16">
         <f>($D$15*((1-RR)*$H$14-(1-RR+$B$15*C18/10000)*$H$15))</f>
-        <v>2.3041457483617407E-3</v>
-      </c>
-      <c r="N18" s="20">
+        <v>2.3175483401408187E-3</v>
+      </c>
+      <c r="N18" s="16">
         <f>($D$16*((1-RR)*$H$15-(1-RR+$B$16*C18/10000)*$H$16))</f>
-        <v>5.3944809624303838E-3</v>
-      </c>
-      <c r="O18" s="20">
+        <v>5.3751130338677974E-3</v>
+      </c>
+      <c r="O18" s="16">
         <f>($D$17*((1-RR)*$H$16-(1-RR+$B$17*C18/10000)*$H$17))</f>
-        <v>6.9700402756636502E-3</v>
-      </c>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20">
+        <v>6.9218436430963128E-3</v>
+      </c>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16">
         <f t="shared" si="9"/>
-        <v>-9.3681012602926089E-3</v>
-      </c>
-      <c r="S18" s="20">
+        <v>-9.2770291047460235E-3</v>
+      </c>
+      <c r="S18" s="16">
         <f t="shared" si="5"/>
-        <v>0.60005475733613223</v>
-      </c>
-      <c r="T18" s="20">
+        <v>0.58808573949093113</v>
+      </c>
+      <c r="T18" s="16">
         <f t="shared" si="13"/>
-        <v>-1.5612077307546261E-2</v>
-      </c>
-      <c r="U18" s="20">
+        <v>-1.5774960149138397E-2</v>
+      </c>
+      <c r="U18" s="16">
         <f t="shared" si="6"/>
-        <v>0.81712988696531108</v>
+        <v>0.81678425940674526</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="17">
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="25">
         <f>AVERAGE(C18,C20)</f>
         <v>353.2</v>
       </c>
-      <c r="D19" s="19">
-        <v>0.96857779166533953</v>
-      </c>
-      <c r="E19" s="41">
+      <c r="D19" s="15">
+        <v>0.94689889010399997</v>
+      </c>
+      <c r="E19" s="27">
         <f t="shared" si="0"/>
-        <v>6.0374976560801562E-2</v>
-      </c>
-      <c r="F19" s="43">
+        <v>6.0575655501680231E-2</v>
+      </c>
+      <c r="F19" s="29">
         <f t="shared" si="3"/>
-        <v>3.9425351524786989E-2</v>
-      </c>
-      <c r="G19" s="26">
+        <v>3.9604742054686115E-2</v>
+      </c>
+      <c r="G19" s="22">
         <f t="shared" si="1"/>
-        <v>0.23790754186702212</v>
-      </c>
-      <c r="H19" s="28">
+        <v>0.23859544279707923</v>
+      </c>
+      <c r="H19" s="24">
         <f t="shared" si="12"/>
-        <v>0.76209245813297788</v>
-      </c>
-      <c r="I19" s="20">
+        <v>0.76140455720292077</v>
+      </c>
+      <c r="I19" s="16">
         <f t="shared" si="4"/>
-        <v>-1.1802226448168623E-2</v>
-      </c>
-      <c r="J19" s="20">
+        <v>-1.1777983984847022E-2</v>
+      </c>
+      <c r="J19" s="16">
         <f t="shared" si="8"/>
-        <v>-9.727754027020287E-3</v>
-      </c>
-      <c r="K19" s="20">
+        <v>-9.6783130474336638E-3</v>
+      </c>
+      <c r="K19" s="16">
         <f t="shared" si="10"/>
-        <v>-5.5820052395030252E-3</v>
-      </c>
-      <c r="L19" s="20">
+        <v>-5.5266548527959022E-3</v>
+      </c>
+      <c r="L19" s="16">
         <f t="shared" si="11"/>
-        <v>-2.196509029126261E-3</v>
-      </c>
-      <c r="M19" s="20">
+        <v>-2.148456091398986E-3</v>
+      </c>
+      <c r="M19" s="16">
         <f>($D$15*((1-RR)*$H$14-(1-RR+$B$15*C19/10000)*$H$15))</f>
-        <v>1.0763299718495468E-3</v>
-      </c>
-      <c r="N19" s="20">
+        <v>1.1053231621571719E-3</v>
+      </c>
+      <c r="N19" s="16">
         <f>($D$16*((1-RR)*$H$15-(1-RR+$B$16*C19/10000)*$H$16))</f>
-        <v>4.2158519440759013E-3</v>
-      </c>
-      <c r="O19" s="20">
+        <v>4.2144906672587192E-3</v>
+      </c>
+      <c r="O19" s="16">
         <f>($D$17*((1-RR)*$H$16-(1-RR+$B$17*C19/10000)*$H$17))</f>
-        <v>5.8430624631651187E-3</v>
-      </c>
-      <c r="P19" s="20">
+        <v>5.8150153444785522E-3</v>
+      </c>
+      <c r="P19" s="16">
         <f>($D$18*((1-RR)*$H$17-(1-RR+$B$18*C19/10000)*$H$18))</f>
-        <v>8.2969937757526504E-3</v>
-      </c>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20">
+        <v>8.2279525041128697E-3</v>
+      </c>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16">
         <f t="shared" si="9"/>
-        <v>-9.8762565889749816E-3</v>
-      </c>
-      <c r="S19" s="20">
+        <v>-9.7686262984682595E-3</v>
+      </c>
+      <c r="S19" s="16">
         <f t="shared" si="5"/>
-        <v>0.59825175880001358</v>
-      </c>
-      <c r="T19" s="20">
+        <v>0.58486156846163662</v>
+      </c>
+      <c r="T19" s="16">
         <f t="shared" si="13"/>
-        <v>-1.6508529132927236E-2</v>
-      </c>
-      <c r="U19" s="20">
+        <v>-1.6702458881274609E-2</v>
+      </c>
+      <c r="U19" s="16">
         <f t="shared" si="6"/>
-        <v>0.7786009872659051</v>
+        <v>0.77810701608419541</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="17">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="13">
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="19">
         <v>380.65</v>
       </c>
-      <c r="D20" s="19">
-        <v>0.9630440739465842</v>
-      </c>
-      <c r="E20" s="41">
+      <c r="D20" s="15">
+        <v>0.93918722794499998</v>
+      </c>
+      <c r="E20" s="27">
         <f t="shared" si="0"/>
-        <v>6.5590975003326585E-2</v>
-      </c>
-      <c r="F20" s="42">
+        <v>6.5842402988677398E-2</v>
+      </c>
+      <c r="F20" s="28">
         <f t="shared" si="3"/>
-        <v>4.1696931324958331E-2</v>
-      </c>
-      <c r="G20" s="26">
+        <v>4.1914099356345047E-2</v>
+      </c>
+      <c r="G20" s="22">
         <f t="shared" si="1"/>
-        <v>0.27960447319198045</v>
-      </c>
-      <c r="H20" s="26">
+        <v>0.28050954215342427</v>
+      </c>
+      <c r="H20" s="22">
         <f t="shared" si="12"/>
-        <v>0.72039552680801955</v>
-      </c>
-      <c r="I20" s="20">
+        <v>0.71949045784657573</v>
+      </c>
+      <c r="I20" s="16">
         <f t="shared" si="4"/>
-        <v>-1.3158889413002021E-2</v>
-      </c>
-      <c r="J20" s="20">
+        <v>-1.3131860284612674E-2</v>
+      </c>
+      <c r="J20" s="16">
         <f t="shared" si="8"/>
-        <v>-1.1064423624024025E-2</v>
-      </c>
-      <c r="K20" s="20">
+        <v>-1.1008551743503047E-2</v>
+      </c>
+      <c r="K20" s="16">
         <f t="shared" si="10"/>
-        <v>-6.8894468302746108E-3</v>
-      </c>
-      <c r="L20" s="20">
+        <v>-6.8242731611503609E-3</v>
+      </c>
+      <c r="L20" s="16">
         <f t="shared" si="11"/>
-        <v>-3.4674613735872352E-3</v>
-      </c>
-      <c r="M20" s="20">
+        <v>-3.4065966418340039E-3</v>
+      </c>
+      <c r="M20" s="16">
         <f>($D$15*((1-RR)*$H$14-(1-RR+$B$15*C20/10000)*$H$15))</f>
-        <v>-1.5148580466264717E-4</v>
-      </c>
-      <c r="N20" s="20">
+        <v>-1.0690201582647507E-4</v>
+      </c>
+      <c r="N20" s="16">
         <f>($D$16*((1-RR)*$H$15-(1-RR+$B$16*C20/10000)*$H$16))</f>
-        <v>3.0372229257215272E-3</v>
-      </c>
-      <c r="O20" s="20">
+        <v>3.0538683006497477E-3</v>
+      </c>
+      <c r="O20" s="16">
         <f>($D$17*((1-RR)*$H$16-(1-RR+$B$17*C20/10000)*$H$17))</f>
-        <v>4.716084650666588E-3</v>
-      </c>
-      <c r="P20" s="20">
+        <v>4.7081870458606841E-3</v>
+      </c>
+      <c r="P20" s="16">
         <f>($D$18*((1-RR)*$H$17-(1-RR+$B$18*C20/10000)*$H$18))</f>
-        <v>7.2258862912127683E-3</v>
-      </c>
-      <c r="Q20" s="20">
+        <v>7.1788759034797757E-3</v>
+      </c>
+      <c r="Q20" s="16">
         <f>($D$19*((1-RR)*$H$18-(1-RR+$B$19*C20/10000)*$H$19))</f>
-        <v>8.8631514371033306E-3</v>
-      </c>
-      <c r="R20" s="20">
+        <v>8.7790906773571823E-3</v>
+      </c>
+      <c r="R20" s="16">
         <f t="shared" si="9"/>
-        <v>-1.0889361740846324E-2</v>
-      </c>
-      <c r="S20" s="20">
+        <v>-1.0758161919579167E-2</v>
+      </c>
+      <c r="S20" s="16">
         <f t="shared" si="5"/>
-        <v>0.59615558070533892</v>
-      </c>
-      <c r="T20" s="20">
+        <v>0.58138741768286317</v>
+      </c>
+      <c r="T20" s="16">
         <f t="shared" si="13"/>
-        <v>-1.8265972999804217E-2</v>
-      </c>
-      <c r="U20" s="20">
+        <v>-1.8504290929542543E-2</v>
+      </c>
+      <c r="U20" s="16">
         <f t="shared" si="6"/>
-        <v>0.73866149980782381</v>
+        <v>0.73799474877611826</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+      <c r="A23" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
@@ -2709,8 +2625,8 @@
       <c r="C24" s="1">
         <v>114.4</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
       <c r="G24" s="1">
         <v>18.34</v>
       </c>
@@ -2722,8 +2638,8 @@
       <c r="C25" s="1">
         <v>133.77000000000001</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
       <c r="G25" s="1">
         <v>20.82</v>
       </c>
@@ -2735,8 +2651,8 @@
       <c r="C26" s="1">
         <v>200.59</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
       <c r="G26" s="1">
         <v>35.69</v>
       </c>
@@ -2748,8 +2664,8 @@
       <c r="C27" s="1">
         <v>267.33999999999997</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
       <c r="G27" s="1">
         <v>49.01</v>
       </c>
@@ -2761,22 +2677,22 @@
       <c r="C28" s="1">
         <v>325.75</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="G28" s="1">
         <v>66.540000000000006</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="1">
         <v>380.65</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
       <c r="G29" s="2">
         <v>81.91</v>
       </c>
@@ -2788,8 +2704,8 @@
       <c r="C30" s="1">
         <v>424.28</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
       <c r="G30" s="1">
         <v>106.74</v>
       </c>
@@ -2801,8 +2717,8 @@
       <c r="C31" s="1">
         <v>450.55</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
       <c r="G31" s="1">
         <v>127.1</v>
       </c>
@@ -2814,8 +2730,8 @@
       <c r="C32" s="1">
         <v>464.43</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
       <c r="G32" s="1">
         <v>138.04</v>
       </c>
@@ -2827,8 +2743,8 @@
       <c r="C33" s="1">
         <v>467.65</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
       <c r="G33" s="1">
         <v>141.33000000000001</v>
       </c>
@@ -2844,300 +2760,387 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" style="39" customWidth="1"/>
-    <col min="2" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="30">
+        <v>0</v>
+      </c>
+      <c r="B2" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C10</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>'BOOTSTRAP EXAMPLE'!D10</f>
         <v>1</v>
       </c>
-      <c r="C4" s="6">
-        <v>5.9999999999999991</v>
-      </c>
-      <c r="D4" s="6">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6">
-        <v>17.999999999999993</v>
-      </c>
-      <c r="F4" s="6">
-        <v>23.999999999999989</v>
-      </c>
-      <c r="G4" s="6">
-        <v>30</v>
-      </c>
-      <c r="H4" s="6">
-        <v>36.000000000000014</v>
-      </c>
-      <c r="I4" s="6">
-        <v>42.000000000000021</v>
-      </c>
-      <c r="J4" s="6">
-        <v>48.000000000000028</v>
-      </c>
-      <c r="K4" s="6">
-        <v>54.000000000000014</v>
-      </c>
-      <c r="L4" s="6">
-        <v>59.999999999999986</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
-        <v>23</v>
+      <c r="D2">
+        <f>'BOOTSTRAP EXAMPLE'!E10</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>'BOOTSTRAP EXAMPLE'!F10</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>'BOOTSTRAP EXAMPLE'!H10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C11</f>
+        <v>114.4</v>
+      </c>
+      <c r="C3">
+        <f>'BOOTSTRAP EXAMPLE'!D11</f>
+        <v>0.99583479331400004</v>
+      </c>
+      <c r="D3">
+        <f>'BOOTSTRAP EXAMPLE'!E11</f>
+        <v>1.8976355744616674E-2</v>
+      </c>
+      <c r="E3">
+        <f>'BOOTSTRAP EXAMPLE'!F11</f>
+        <v>9.4433071386118561E-3</v>
+      </c>
+      <c r="F3">
+        <f>'BOOTSTRAP EXAMPLE'!H11</f>
+        <v>0.99055669286138814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
+        <v>1</v>
+      </c>
+      <c r="B4" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C12</f>
+        <v>133.77000000000001</v>
+      </c>
+      <c r="C4">
+        <f>'BOOTSTRAP EXAMPLE'!D12</f>
+        <v>0.99096300549399996</v>
+      </c>
+      <c r="D4">
+        <f>'BOOTSTRAP EXAMPLE'!E12</f>
+        <v>2.2197421712663361E-2</v>
+      </c>
+      <c r="E4">
+        <f>'BOOTSTRAP EXAMPLE'!F12</f>
+        <v>1.2509564610413304E-2</v>
+      </c>
+      <c r="F4">
+        <f>'BOOTSTRAP EXAMPLE'!H12</f>
+        <v>0.97804712825097484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="30">
+        <v>1.5</v>
       </c>
       <c r="B5" s="31">
-        <v>0</v>
-      </c>
-      <c r="C5" s="31">
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="D5" s="31">
-        <v>1</v>
-      </c>
-      <c r="E5" s="31">
-        <v>1.4999999999999996</v>
-      </c>
-      <c r="F5" s="31">
-        <v>1.9999999999999991</v>
-      </c>
-      <c r="G5" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C13</f>
+        <v>167.18</v>
+      </c>
+      <c r="C5">
+        <f>'BOOTSTRAP EXAMPLE'!D13</f>
+        <v>0.98569666301900005</v>
+      </c>
+      <c r="D5">
+        <f>'BOOTSTRAP EXAMPLE'!E13</f>
+        <v>2.7797843343853341E-2</v>
+      </c>
+      <c r="E5">
+        <f>'BOOTSTRAP EXAMPLE'!F13</f>
+        <v>1.8886540726516965E-2</v>
+      </c>
+      <c r="F5">
+        <f>'BOOTSTRAP EXAMPLE'!H13</f>
+        <v>0.95916058752445787</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="30">
+        <v>2</v>
+      </c>
+      <c r="B6" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C14</f>
+        <v>200.59</v>
+      </c>
+      <c r="C6">
+        <f>'BOOTSTRAP EXAMPLE'!D14</f>
+        <v>0.98010503953600003</v>
+      </c>
+      <c r="D6">
+        <f>'BOOTSTRAP EXAMPLE'!E14</f>
+        <v>3.3451743598432469E-2</v>
+      </c>
+      <c r="E6">
+        <f>'BOOTSTRAP EXAMPLE'!F14</f>
+        <v>2.3875123521640451E-2</v>
+      </c>
+      <c r="F6">
+        <f>'BOOTSTRAP EXAMPLE'!H14</f>
+        <v>0.93528546400281742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="30">
         <v>2.5</v>
       </c>
-      <c r="H5" s="31">
-        <v>3.0000000000000009</v>
-      </c>
-      <c r="I5" s="31">
-        <v>3.5000000000000018</v>
-      </c>
-      <c r="J5" s="31">
-        <v>4.0000000000000027</v>
-      </c>
-      <c r="K5" s="31">
-        <v>4.5000000000000009</v>
-      </c>
-      <c r="L5" s="31">
-        <v>4.9999999999999991</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32">
-        <v>41059</v>
-      </c>
-      <c r="B6" s="33">
-        <v>0.46137033416414602</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0.42354687411299291</v>
-      </c>
-      <c r="D6" s="33">
-        <v>0.42598092477913829</v>
-      </c>
-      <c r="E6" s="33">
-        <v>0.45950347957462762</v>
-      </c>
-      <c r="F6" s="33">
-        <v>0.50187577217048662</v>
-      </c>
-      <c r="G6" s="33">
-        <v>0.54450723791059019</v>
-      </c>
-      <c r="H6" s="33">
-        <v>0.58574185700581216</v>
-      </c>
-      <c r="I6" s="33">
-        <v>0.62631573124380424</v>
-      </c>
-      <c r="J6" s="33">
-        <v>0.66731655383960786</v>
-      </c>
-      <c r="K6" s="33">
-        <v>0.70947727908008651</v>
-      </c>
-      <c r="L6" s="33">
-        <v>0.75312201786420929</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="34">
-        <f>B6/100</f>
-        <v>4.6137033416414602E-3</v>
-      </c>
-      <c r="C7" s="34">
-        <f>C6/100</f>
-        <v>4.2354687411299292E-3</v>
-      </c>
-      <c r="D7" s="34">
-        <f t="shared" ref="D7:L7" si="0">D6/100</f>
-        <v>4.2598092477913827E-3</v>
-      </c>
-      <c r="E7" s="34">
+      <c r="B7" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C15</f>
+        <v>233.96499999999997</v>
+      </c>
+      <c r="C7">
+        <f>'BOOTSTRAP EXAMPLE'!D15</f>
+        <v>0.97410111162099999</v>
+      </c>
+      <c r="D7">
+        <f>'BOOTSTRAP EXAMPLE'!E15</f>
+        <v>3.9174425426960563E-2</v>
+      </c>
+      <c r="E7">
+        <f>'BOOTSTRAP EXAMPLE'!F15</f>
+        <v>2.8578590499201306E-2</v>
+      </c>
+      <c r="F7">
+        <f>'BOOTSTRAP EXAMPLE'!H15</f>
+        <v>0.90670687350361612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="30">
+        <v>3</v>
+      </c>
+      <c r="B8" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C16</f>
+        <v>267.33999999999997</v>
+      </c>
+      <c r="C8">
+        <f>'BOOTSTRAP EXAMPLE'!D16</f>
+        <v>0.96783236118000004</v>
+      </c>
+      <c r="D8">
+        <f>'BOOTSTRAP EXAMPLE'!E16</f>
+        <v>4.4993707639747055E-2</v>
+      </c>
+      <c r="E8">
+        <f>'BOOTSTRAP EXAMPLE'!F16</f>
+        <v>3.2974468454083694E-2</v>
+      </c>
+      <c r="F8">
+        <f>'BOOTSTRAP EXAMPLE'!H16</f>
+        <v>0.87373240504953242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C17</f>
+        <v>296.54499999999996</v>
+      </c>
+      <c r="C9">
+        <f>'BOOTSTRAP EXAMPLE'!D17</f>
+        <v>0.96123247030000003</v>
+      </c>
+      <c r="D9">
+        <f>'BOOTSTRAP EXAMPLE'!E17</f>
+        <v>5.0170389471591678E-2</v>
+      </c>
+      <c r="E9">
+        <f>'BOOTSTRAP EXAMPLE'!F17</f>
+        <v>3.4775856267641569E-2</v>
+      </c>
+      <c r="F9">
+        <f>'BOOTSTRAP EXAMPLE'!H17</f>
+        <v>0.83895654878189085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>4</v>
+      </c>
+      <c r="B10" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C18</f>
+        <v>325.75</v>
+      </c>
+      <c r="C10">
+        <f>'BOOTSTRAP EXAMPLE'!D18</f>
+        <v>0.95423927873100001</v>
+      </c>
+      <c r="D10">
+        <f>'BOOTSTRAP EXAMPLE'!E18</f>
+        <v>5.5470680605277427E-2</v>
+      </c>
+      <c r="E10">
+        <f>'BOOTSTRAP EXAMPLE'!F18</f>
+        <v>3.7947249524283966E-2</v>
+      </c>
+      <c r="F10">
+        <f>'BOOTSTRAP EXAMPLE'!H18</f>
+        <v>0.80100929925760689</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="30">
+        <v>4.5</v>
+      </c>
+      <c r="B11" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C19</f>
+        <v>353.2</v>
+      </c>
+      <c r="C11">
+        <f>'BOOTSTRAP EXAMPLE'!D19</f>
+        <v>0.94689889010399997</v>
+      </c>
+      <c r="D11">
+        <f>'BOOTSTRAP EXAMPLE'!E19</f>
+        <v>6.0575655501680231E-2</v>
+      </c>
+      <c r="E11">
+        <f>'BOOTSTRAP EXAMPLE'!F19</f>
+        <v>3.9604742054686115E-2</v>
+      </c>
+      <c r="F11">
+        <f>'BOOTSTRAP EXAMPLE'!H19</f>
+        <v>0.76140455720292077</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="30">
+        <v>5</v>
+      </c>
+      <c r="B12" s="31">
+        <f>'BOOTSTRAP EXAMPLE'!C20</f>
+        <v>380.65</v>
+      </c>
+      <c r="C12">
+        <f>'BOOTSTRAP EXAMPLE'!D20</f>
+        <v>0.93918722794499998</v>
+      </c>
+      <c r="D12">
+        <f>'BOOTSTRAP EXAMPLE'!E20</f>
+        <v>6.5842402988677398E-2</v>
+      </c>
+      <c r="E12">
+        <f>'BOOTSTRAP EXAMPLE'!F20</f>
+        <v>4.1914099356345047E-2</v>
+      </c>
+      <c r="F12">
+        <f>'BOOTSTRAP EXAMPLE'!H20</f>
+        <v>0.71949045784657573</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f>A1&amp;","&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;","&amp;E1&amp;","&amp;F1</f>
+        <v>Tenor,CDS,DF,Lambda,PD,P</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2</f>
+        <v>0,0,1,0,0,1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f t="shared" ref="A17:A25" si="0">A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3</f>
+        <v>0.5,114.4,0.995834793314,0.0189763557446167,0.00944330713861186,0.990556692861388</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>4.5950347957462757E-3</v>
-      </c>
-      <c r="F7" s="34">
+        <v>1,133.77,0.990963005494,0.0221974217126634,0.0125095646104133,0.978047128250975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>5.0187577217048664E-3</v>
-      </c>
-      <c r="G7" s="34">
+        <v>1.5,167.18,0.985696663019,0.0277978433438533,0.018886540726517,0.959160587524458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>5.4450723791059016E-3</v>
-      </c>
-      <c r="H7" s="34">
+        <v>2,200.59,0.980105039536,0.0334517435984325,0.0238751235216405,0.935285464002817</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>5.8574185700581219E-3</v>
-      </c>
-      <c r="I7" s="34">
+        <v>2.5,233.965,0.974101111621,0.0391744254269606,0.0285785904992013,0.906706873503616</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>6.2631573124380426E-3</v>
-      </c>
-      <c r="J7" s="34">
+        <v>3,267.34,0.96783236118,0.0449937076397471,0.0329744684540837,0.873732405049532</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>6.6731655383960786E-3</v>
-      </c>
-      <c r="K7" s="34">
+        <v>3.5,296.545,0.9612324703,0.0501703894715917,0.0347758562676416,0.838956548781891</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>7.094772790800865E-3</v>
-      </c>
-      <c r="L7" s="34">
+        <v>4,325.75,0.954239278731,0.0554706806052774,0.037947249524284,0.801009299257607</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>7.5312201786420932E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="35">
-        <v>1</v>
-      </c>
-      <c r="C8" s="35">
-        <f>EXP(-C7*(C5-$B$5))</f>
-        <v>0.9978845064467694</v>
-      </c>
-      <c r="D8" s="35">
-        <f t="shared" ref="D8:L8" si="1">EXP(-D7*(D5-$B$5))</f>
-        <v>0.99574925087026533</v>
-      </c>
-      <c r="E8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.99313114696376492</v>
-      </c>
-      <c r="F8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.99001269228735078</v>
-      </c>
-      <c r="G8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.98647955260389597</v>
-      </c>
-      <c r="H8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.98258123599502745</v>
-      </c>
-      <c r="I8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.97831746958591959</v>
-      </c>
-      <c r="J8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.97366043824697446</v>
-      </c>
-      <c r="K8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.96857779166533953</v>
-      </c>
-      <c r="L8" s="35">
-        <f t="shared" si="1"/>
-        <v>0.9630440739465842</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="35">
-        <f>B8</f>
-        <v>1</v>
-      </c>
-      <c r="C9" s="35">
-        <f>C8/B8</f>
-        <v>0.9978845064467694</v>
-      </c>
-      <c r="D9" s="35">
-        <f t="shared" ref="D9:L9" si="2">D8/C8</f>
-        <v>0.99786021772789402</v>
-      </c>
-      <c r="E9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99737071968247804</v>
-      </c>
-      <c r="F9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.9968599769668407</v>
-      </c>
-      <c r="G9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99643121779045907</v>
-      </c>
-      <c r="H9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99604825401745167</v>
-      </c>
-      <c r="I9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99566064743258598</v>
-      </c>
-      <c r="J9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99523975449307245</v>
-      </c>
-      <c r="K9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99477985714322958</v>
-      </c>
-      <c r="L9" s="35">
-        <f t="shared" si="2"/>
-        <v>0.99428675965278857</v>
+        <v>4.5,353.2,0.946898890104,0.0605756555016802,0.0396047420546861,0.761404557202921</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>A12&amp;","&amp;B12&amp;","&amp;C12&amp;","&amp;D12&amp;","&amp;E12&amp;","&amp;F12</f>
+        <v>5,380.65,0.939187227945,0.0658424029886774,0.041914099356345,0.719490457846576</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>